<commit_message>
- just updated a new xlsx test file 2 quick land jobs
</commit_message>
<xml_diff>
--- a/autoast/2_quick_land_jobs.xlsx
+++ b/autoast/2_quick_land_jobs.xlsx
@@ -602,7 +602,11 @@
           <t>True</t>
         </is>
       </c>
-      <c r="M2" s="4" t="n"/>
+      <c r="M2" s="4" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
       <c r="N2" s="10" t="n">
         <v>876372</v>
       </c>
@@ -651,7 +655,7 @@
       </c>
       <c r="M3" s="4" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N3" s="10" t="n">

</xml_diff>